<commit_message>
changes for the unix systems
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -489,22 +489,22 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>ДГИ-В-86378/24  09.08.2024</t>
+          <t>ДГИ-В-87616/24  14.08.2024</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ДГИ-В-86378/24 09.08.2024</t>
+          <t>ДГИ-В-87616/24 14.08.2024</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Кому: Пахмутов С.А. (Департамент городского имущества города Москвы), Курзина Ю.А. (Департамент городского имущества города Москвы), Мусиенко О.А. (Департамент городского имущества города Москвы), Николаев А.В. (Департамент городского имущества города Москвы), Дмитриева Н.В. (Департамент городского имущества города Москвы)  От кого:  Спесивцева С.В. (Департамент городского имущества города Москвы)</t>
+          <t>Кому: Мусиенко О.А. (Департамент городского имущества города Москвы)  От кого:  Демонова Л.В. (Департамент городского имущества города Москвы)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>УПОЖС. Анадырский проезд, д. 27, кв. 79, ком. № 2</t>
+          <t>О показе жилых помещений ЮВАО</t>
         </is>
       </c>
     </row>
@@ -517,27 +517,27 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Вх</t>
+          <t>Вн</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ДГИ-1-44165/24  09.08.2024</t>
+          <t>ДГИ-В-87613/24  14.08.2024</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>07-5786/2024 01.08.2024</t>
+          <t>ДГИ-В-87613/24 14.08.2024</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Дусеев Н.В. (Управление Федеральной службы государственной регистрации, кадастра и картографии по Москве)</t>
+          <t>Кому: Мусиенко О.А. (Департамент городского имущества города Москвы)  От кого:  Демонова Л.В. (Департамент городского имущества города Москвы)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>ДГИ-238588/24-(0)-0 Запрос сведений по объекту с кн 77:17:0100211:1163</t>
+          <t>Об осмотре жилых помещений по КПИ и ДСН в ЮВАО</t>
         </is>
       </c>
     </row>
@@ -555,22 +555,22 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ДГИ-1-44161/24  09.08.2024</t>
+          <t>ДГИ-1-44675/24  13.08.2024</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>6 01.08.2024</t>
+          <t>4 02.08.2024</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Голев А.А. (Финансовый управляющий)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Ермоленко Н.В. (Финансовый управляющий)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>ДГИ-238527/24-(0)-0 Запрос по делу №А40-91776/24</t>
+          <t>ДГИ-241024/24-(0)-0 запрос по делу А40-95663/2024</t>
         </is>
       </c>
     </row>
@@ -588,22 +588,22 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>ДГИ-Э-127121/24  09.08.2024</t>
+          <t>ДГИ-1-44670/24  13.08.2024</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>07-6020/2024 09.08.2024</t>
+          <t>2 05.08.2024</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Липнухов М.А. (Управление Федеральной службы государственной регистрации, кадастра и картографии по Москве)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Мокрушин С.В. (Конкурсный управляющий)</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>О направлении информации в отношении объекта недвижимого имущества с кн 77:03:0010009:3129</t>
+          <t>ДГИ-241090/24-(0)-0 запрос по делу А40-287374/23</t>
         </is>
       </c>
     </row>
@@ -621,22 +621,22 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ДГИ-1-44140/24  09.08.2024</t>
+          <t>ДГИ-1-44664/24  13.08.2024</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3 25.07.2024</t>
+          <t>Б/Н 02.08.2024</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Крашенинникова А.В. ("Финансовый управляющий")</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Алехин Н.Н. (Конкурсный управляющий)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>ДГИ-238497/24-(0)-0 запрос по делу А40-223662/2023</t>
+          <t>ДГИ-240927/24-(0)-0 запрос по делу А40-169117/23</t>
         </is>
       </c>
     </row>
@@ -654,22 +654,22 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>ДГИ-1-44137/24  09.08.2024</t>
+          <t>ДГИ-1-44660/24  13.08.2024</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>3 01.08.2024</t>
+          <t>9 02.08.2024</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Кулешина М.Е. (Финансовый управляющий)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Курзин Д.А. (Финансовый управляющий)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>ДГИ-238495/24-(0)-0 запрос по делу А40-106313/2024</t>
+          <t>ДГИ-240954/24-(0)-0 запрос по делу А40-111870/2024</t>
         </is>
       </c>
     </row>
@@ -687,22 +687,22 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>ДГИ-1-44132/24  09.08.2024</t>
+          <t>ДГИ-1-44658/24  13.08.2024</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>4 29.07.2024</t>
+          <t>1 04.06.2024</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Махно В.А. ("Финансовый управляющий")</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Вахрушев В.О. (Временный управляющий)</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>ДГИ-238489/24-(0)-0 запрос по делу А40-159526/201-164-430</t>
+          <t>ДГИ-240946/24-(0)-0 запрос по делу А40-79798/24</t>
         </is>
       </c>
     </row>
@@ -720,22 +720,22 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>ДГИ-1-44131/24  09.08.2024</t>
+          <t>ДГИ-1-44654/24  13.08.2024</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>12 31.07.2024</t>
+          <t>9 05.08.2024</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Курзин Д.А. (Финансовый управляющий)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Ломакина М.М. (Финансовый управляющий)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>ДГИ-238511/24-(0)-0 Запрос по делу №А40-135129/24</t>
+          <t>ДГИ-241014/24-(0)-0 запрос по делу А40-73286/2024</t>
         </is>
       </c>
     </row>
@@ -753,22 +753,22 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>ДГИ-1-44127/24  09.08.2024</t>
+          <t>ДГИ-1-44650/24  13.08.2024</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2 30.07.2024</t>
+          <t>859-47 07.08.2024</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Котова Е.С. ("Финансовый управляющий")</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Стародубцев А.В. (Конкурсный управляющий)</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>ДГИ-238482/24-(0)-0 запрос по делу А40-47748/24</t>
+          <t>ДГИ-240940/24-(0)-0 запрос по делу А40-253586/23</t>
         </is>
       </c>
     </row>
@@ -781,27 +781,27 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Вх</t>
+          <t>Гр</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>ДГИ-1-44125/24  09.08.2024</t>
+          <t>ДГИ-ЭГР-46848/24  13.08.2024</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>3 02.08.2024</t>
+          <t>56021949 13.08.2024</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Абукаев А.А. ("Финансовый управляющий")</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Обращение граждан (Обращение граждан)</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>ДГИ-238508/24-(0)-0 Запрос по делу №А40-142851/24-105-360ф</t>
+          <t>Обращения граждан Вопрос 1. Сообщение с mos.ru, идентификатор: 56021949 Корякин Анатолий Алексеевич, по очереди</t>
         </is>
       </c>
     </row>
@@ -819,22 +819,22 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>ДГИ-1-44124/24  09.08.2024</t>
+          <t>ДГИ-1-44633/24  13.08.2024</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2 31.07.2024</t>
+          <t>20 06.08.2024</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Котова Е.С. ("Финансовый управляющий")</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Пуртов Н.С. (Финансовый управляющий)</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>ДГИ-238481/24-(0)-0 запрос по делу А40-69402/24</t>
+          <t>ДГИ-240886/24-(0)-0 запрос по делу А40-284028/23</t>
         </is>
       </c>
     </row>
@@ -852,22 +852,22 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>ДГИ-1-44123/24  09.08.2024</t>
+          <t>ДГИ-Э-128678/24  13.08.2024</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>5 01.08.2024</t>
+          <t>А40-137492/2024 13.08.2024</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Морозов М.Н. ("Финансовый управляющий")</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Волкова Л.И. (Финансовый управляющий)</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>ДГИ-238506/24-(0)-0 Запрос по делу №А40-92922/24</t>
+          <t>Запрос по делу №А40-137492/2024</t>
         </is>
       </c>
     </row>
@@ -885,22 +885,22 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>ДГИ-1-44120/24  09.08.2024</t>
+          <t>ДГИ-1-44632/24  13.08.2024</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>4 02.08.2024</t>
+          <t>27 05.08.2024</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Тихомиров Д.С. (Финансовый управляющий)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Феденко А.А. (Финансовый управляющий)</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>ДГИ-238503/24-(0)-0 Запрос по делу №А40-97600/24</t>
+          <t>ДГИ-240884/24-(0)-0 запрос по делу А40-103528/23</t>
         </is>
       </c>
     </row>
@@ -918,22 +918,22 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>ДГИ-1-44118/24  09.08.2024</t>
+          <t>ДГИ-1-44630/24  13.08.2024</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>10 04.08.2024</t>
+          <t>3 29.07.2024</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Мерзляков М.В. ("Финансовый управляющий")</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Слесарев К.И. (Финансовый управляющий)</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>ДГИ-238475/24-(0)-0 запрос по делу А40-112001/24</t>
+          <t>ДГИ-240883/24-(0)-0 запрос по делу А40-116370/24</t>
         </is>
       </c>
     </row>
@@ -946,27 +946,27 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Вх</t>
+          <t>Гр</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>ДГИ-1-44117/24  09.08.2024</t>
+          <t>ДГИ-ЭГР-46845/24  13.08.2024</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>8 01.08.2024</t>
+          <t>56021855 13.08.2024</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Гасанова Н.В. (Финансовый управляющий)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Обращение граждан (Обращение граждан)</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>ДГИ-238498/24-(0)-0 Запрос по делу №А40-116337/24</t>
+          <t>Обращения граждан Вопрос 1. Сообщение с mos.ru, идентификатор: 56021855 Фоломеева Наталья Ивановна, Отказ в принятии на учет нуждающихся в жилых помещениях</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating script for ubuntu on server
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -489,22 +489,22 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>ДГИ-В-87616/24  14.08.2024</t>
+          <t>ДГИ-В-87772/24  14.08.2024</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ДГИ-В-87616/24 14.08.2024</t>
+          <t>ДГИ-В-87772/24 14.08.2024</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Кому: Мусиенко О.А. (Департамент городского имущества города Москвы)  От кого:  Демонова Л.В. (Департамент городского имущества города Москвы)</t>
+          <t>Кому: Мусиенко О.А. (Департамент городского имущества города Москвы)  От кого:  Мишиева Э.Ш. (Департамент городского имущества города Москвы)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>О показе жилых помещений ЮВАО</t>
+          <t>УП. СВАО. Информация в отношении дома по адресу: ул. Молокова, д. 17-19</t>
         </is>
       </c>
     </row>
@@ -517,27 +517,27 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Вн</t>
+          <t>Вх</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ДГИ-В-87613/24  14.08.2024</t>
+          <t>ДГИ-Э-129183/24  14.08.2024</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>ДГИ-В-87613/24 14.08.2024</t>
+          <t>13/2 13.08.2024</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Кому: Мусиенко О.А. (Департамент городского имущества города Москвы)  От кого:  Демонова Л.В. (Департамент городского имущества города Москвы)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  --- ("-")</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Об осмотре жилых помещений по КПИ и ДСН в ЮВАО</t>
+          <t>Запрос в отношении гр. Республики Беларусь Козодавенко А.В.</t>
         </is>
       </c>
     </row>
@@ -550,27 +550,27 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Вх</t>
+          <t>Вн</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ДГИ-1-44675/24  13.08.2024</t>
+          <t>ДГИ-В-87616/24  14.08.2024</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>4 02.08.2024</t>
+          <t>ДГИ-В-87616/24 14.08.2024</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Ермоленко Н.В. (Финансовый управляющий)</t>
+          <t>Кому: Мусиенко О.А. (Департамент городского имущества города Москвы)  От кого:  Демонова Л.В. (Департамент городского имущества города Москвы)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>ДГИ-241024/24-(0)-0 запрос по делу А40-95663/2024</t>
+          <t>О показе жилых помещений ЮВАО</t>
         </is>
       </c>
     </row>
@@ -583,27 +583,27 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Вх</t>
+          <t>Гр</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>ДГИ-1-44670/24  13.08.2024</t>
+          <t>ДГИ-ЭГР-46949/24  14.08.2024</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2 05.08.2024</t>
+          <t>56023306 14.08.2024</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Мокрушин С.В. (Конкурсный управляющий)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Обращение граждан (Обращение граждан)</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>ДГИ-241090/24-(0)-0 запрос по делу А40-287374/23</t>
+          <t>Обращения граждан Вопрос 1. Сообщение с mos.ru, идентификатор: 56023306 Исаев Александр Петрович Жалоба , жилищный учет</t>
         </is>
       </c>
     </row>
@@ -616,27 +616,27 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Вх</t>
+          <t>Вн</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ДГИ-1-44664/24  13.08.2024</t>
+          <t>ДГИ-В-87613/24  14.08.2024</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Б/Н 02.08.2024</t>
+          <t>ДГИ-В-87613/24 14.08.2024</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Алехин Н.Н. (Конкурсный управляющий)</t>
+          <t>Кому: Мусиенко О.А. (Департамент городского имущества города Москвы)  От кого:  Демонова Л.В. (Департамент городского имущества города Москвы)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>ДГИ-240927/24-(0)-0 запрос по делу А40-169117/23</t>
+          <t>Об осмотре жилых помещений по КПИ и ДСН в ЮВАО</t>
         </is>
       </c>
     </row>
@@ -649,27 +649,27 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Вх</t>
+          <t>Вн</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>ДГИ-1-44660/24  13.08.2024</t>
+          <t>ДГИ-В-87745/24  14.08.2024</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>9 02.08.2024</t>
+          <t>ДГИ-В-87745/24 14.08.2024</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Курзин Д.А. (Финансовый управляющий)</t>
+          <t>Кому: Спесивцева С.В. (Департамент городского имущества города Москвы), Мусиенко О.А. (Департамент городского имущества города Москвы)  От кого:  Быкова О.В. (Департамент городского имущества города Москвы)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>ДГИ-240954/24-(0)-0 запрос по делу А40-111870/2024</t>
+          <t>УОКУиРП. Ответ. О регистрации права собственности города Москвы на жилой дом по адресу: г. Москва, г. Зеленоград, ул. Заречная, д. 29.</t>
         </is>
       </c>
     </row>
@@ -687,22 +687,22 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>ДГИ-1-44658/24  13.08.2024</t>
+          <t>ДГИ-Ф-2863/24  14.08.2024</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>1 04.06.2024</t>
+          <t>ДГП-03-7213/24 14.08.2024</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Вахрушев В.О. (Временный управляющий)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы), Валуй А.А. (Департамент градостроительной политики города Москвы), Караванова Н.П. (Департамент градостроительной политики города Москвы), Курилов А.Ф. (Департамент градостроительной политики города Москвы), Торсунов В.Ю. (Департамент жилищно-коммунального хозяйства города Москвы), Беляев А.А. (Департамент капитального ремонта города Москвы), Загрутдинов Р.Р. (Департамент строительства города Москвы), Жидкин В.Ф. (Департамент развития новых территорий города Москвы), Княжевская Ю.В. (Комитет по архитектуре и градостроительству города Москвы), Щербаков И.А. (Комитет города Москвы по ценовой политике в строительстве и государственной экспертизе проектов), Слободчиков А.О. (Комитет государственного строительного надзора города Москвы)  От кого:  Стулов Д.Ю. (Департамент градостроительной политики города Москвы)</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>ДГИ-240946/24-(0)-0 запрос по делу А40-79798/24</t>
+          <t>ФАКСОГРАММА 14 августа 2024 года в 13 часов 00 минут в Департаменте градостроительной политики города Москвы в режиме ВКС состоится совещание по вопросу включения в государственные программы города Москвы «Жилище» и «Градостроительная политика» ключевых показателей, характеризующих эффективность от реализации стратегических задач. Ссылка для участия в совещании: https://vks.dgp.mos.ru/c/70601</t>
         </is>
       </c>
     </row>
@@ -715,27 +715,27 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Вх</t>
+          <t>Гр</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>ДГИ-1-44654/24  13.08.2024</t>
+          <t>ДГИ-ЭГР-46931/24  14.08.2024</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>9 05.08.2024</t>
+          <t>56022495 13.08.2024</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Ломакина М.М. (Финансовый управляющий)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Обращение граждан (Обращение граждан)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>ДГИ-241014/24-(0)-0 запрос по делу А40-73286/2024</t>
+          <t>Обращения граждан Вопрос 1. Сообщение с mos.ru, идентификатор: 56022495 Талызин Александр Викторович, Об уведомлении об улучшении жилищных условий</t>
         </is>
       </c>
     </row>
@@ -753,22 +753,22 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>ДГИ-1-44650/24  13.08.2024</t>
+          <t>ДГИ-1-44675/24  13.08.2024</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>859-47 07.08.2024</t>
+          <t>4 02.08.2024</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Стародубцев А.В. (Конкурсный управляющий)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Ермоленко Н.В. (Финансовый управляющий)</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>ДГИ-240940/24-(0)-0 запрос по делу А40-253586/23</t>
+          <t>ДГИ-241024/24-(0)-0 запрос по делу А40-95663/2024</t>
         </is>
       </c>
     </row>
@@ -781,27 +781,27 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Гр</t>
+          <t>Вх</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>ДГИ-ЭГР-46848/24  13.08.2024</t>
+          <t>ДГИ-1-44670/24  13.08.2024</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>56021949 13.08.2024</t>
+          <t>2 05.08.2024</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Обращение граждан (Обращение граждан)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Мокрушин С.В. (Конкурсный управляющий)</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Обращения граждан Вопрос 1. Сообщение с mos.ru, идентификатор: 56021949 Корякин Анатолий Алексеевич, по очереди</t>
+          <t>ДГИ-241090/24-(0)-0 запрос по делу А40-287374/23</t>
         </is>
       </c>
     </row>
@@ -819,22 +819,22 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>ДГИ-1-44633/24  13.08.2024</t>
+          <t>ДГИ-1-44664/24  13.08.2024</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>20 06.08.2024</t>
+          <t>Б/Н 02.08.2024</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Пуртов Н.С. (Финансовый управляющий)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Алехин Н.Н. (Конкурсный управляющий)</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>ДГИ-240886/24-(0)-0 запрос по делу А40-284028/23</t>
+          <t>ДГИ-240927/24-(0)-0 запрос по делу А40-169117/23</t>
         </is>
       </c>
     </row>
@@ -852,22 +852,22 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>ДГИ-Э-128678/24  13.08.2024</t>
+          <t>ДГИ-1-44660/24  13.08.2024</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>А40-137492/2024 13.08.2024</t>
+          <t>9 02.08.2024</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Волкова Л.И. (Финансовый управляющий)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Курзин Д.А. (Финансовый управляющий)</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Запрос по делу №А40-137492/2024</t>
+          <t>ДГИ-240954/24-(0)-0 запрос по делу А40-111870/2024</t>
         </is>
       </c>
     </row>
@@ -885,22 +885,22 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>ДГИ-1-44632/24  13.08.2024</t>
+          <t>ДГИ-1-44658/24  13.08.2024</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>27 05.08.2024</t>
+          <t>1 04.06.2024</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Феденко А.А. (Финансовый управляющий)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Вахрушев В.О. (Временный управляющий)</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>ДГИ-240884/24-(0)-0 запрос по делу А40-103528/23</t>
+          <t>ДГИ-240946/24-(0)-0 запрос по делу А40-79798/24</t>
         </is>
       </c>
     </row>
@@ -918,22 +918,22 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>ДГИ-1-44630/24  13.08.2024</t>
+          <t>ДГИ-1-44654/24  13.08.2024</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>3 29.07.2024</t>
+          <t>9 05.08.2024</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Слесарев К.И. (Финансовый управляющий)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Ломакина М.М. (Финансовый управляющий)</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>ДГИ-240883/24-(0)-0 запрос по делу А40-116370/24</t>
+          <t>ДГИ-241014/24-(0)-0 запрос по делу А40-73286/2024</t>
         </is>
       </c>
     </row>
@@ -946,27 +946,27 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Гр</t>
+          <t>Вх</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>ДГИ-ЭГР-46845/24  13.08.2024</t>
+          <t>ДГИ-1-44650/24  13.08.2024</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>56021855 13.08.2024</t>
+          <t>859-47 07.08.2024</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Обращение граждан (Обращение граждан)</t>
+          <t>Кому: Гаман М.Ф. (Департамент городского имущества города Москвы)  От кого:  Стародубцев А.В. (Конкурсный управляющий)</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Обращения граждан Вопрос 1. Сообщение с mos.ru, идентификатор: 56021855 Фоломеева Наталья Ивановна, Отказ в принятии на учет нуждающихся в жилых помещениях</t>
+          <t>ДГИ-240940/24-(0)-0 запрос по делу А40-253586/23</t>
         </is>
       </c>
     </row>

</xml_diff>